<commit_message>
removed insertion of duplicates into queue status
</commit_message>
<xml_diff>
--- a/SpicePremix.xlsx
+++ b/SpicePremix.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77DD333-1A3F-4C6D-BCE2-331254360AD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B03277B-8BE6-46DB-82E2-E7E50D963F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E1A821C3-D5CF-4798-8FBF-84782CA853F1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="163">
   <si>
     <t>Salt Mix for Fresh Sausage [L]</t>
   </si>
@@ -489,78 +489,6 @@
   </si>
   <si>
     <t>Chocolate Brown Food Colour</t>
-  </si>
-  <si>
-    <t>Gels &amp; emulsions</t>
-  </si>
-  <si>
-    <t>1230G41</t>
-  </si>
-  <si>
-    <t>G2150</t>
-  </si>
-  <si>
-    <t>G8901</t>
-  </si>
-  <si>
-    <t>Ice for Production</t>
-  </si>
-  <si>
-    <t>1230G42</t>
-  </si>
-  <si>
-    <t>G2159</t>
-  </si>
-  <si>
-    <t>G2001</t>
-  </si>
-  <si>
-    <t>Minced Bck/Sft/Ckg/Bef/Fla Fat</t>
-  </si>
-  <si>
-    <t>G2005</t>
-  </si>
-  <si>
-    <t>Minced Lean Pork</t>
-  </si>
-  <si>
-    <t>G2045</t>
-  </si>
-  <si>
-    <t>Minced Imp Lean Pork 4 Sausage</t>
-  </si>
-  <si>
-    <t>G2008</t>
-  </si>
-  <si>
-    <t>Minced Semi Lean</t>
-  </si>
-  <si>
-    <t>G2011</t>
-  </si>
-  <si>
-    <t>Minced Lean Beef</t>
-  </si>
-  <si>
-    <t>H231034</t>
-  </si>
-  <si>
-    <t>Special Bakery Compound</t>
-  </si>
-  <si>
-    <t>Fat Emul. Mix - Smokies (FH)</t>
-  </si>
-  <si>
-    <t>1230G50</t>
-  </si>
-  <si>
-    <t>G21521</t>
-  </si>
-  <si>
-    <t>H231072</t>
-  </si>
-  <si>
-    <t>Beef Fat (Slio Dry Blend 803529)</t>
   </si>
   <si>
     <t>process</t>
@@ -636,7 +564,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -646,12 +574,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -669,7 +591,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -709,15 +631,6 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1095,11 +1008,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{480CE248-70DE-4C88-820C-D422FDAB8229}">
-  <dimension ref="A1:L166"/>
+  <dimension ref="A1:L149"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F153" sqref="F153:F161"/>
+      <selection pane="bottomLeft" activeCell="A150" sqref="A150:XFD166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1119,40 +1032,40 @@
   <sheetData>
     <row r="1" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>175</v>
+        <v>151</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>177</v>
+        <v>153</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>178</v>
+        <v>154</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>180</v>
+        <v>156</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>181</v>
+        <v>157</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>183</v>
+        <v>159</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>184</v>
+        <v>160</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>185</v>
+        <v>161</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>186</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -6293,613 +6206,6 @@
       <c r="J149" s="7"/>
       <c r="K149" s="9"/>
       <c r="L149" s="4"/>
-    </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A150" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="B150" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="C150" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="D150" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="E150" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F150" s="4">
-        <v>100</v>
-      </c>
-      <c r="G150" s="6">
-        <v>2055</v>
-      </c>
-      <c r="H150" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="I150" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="J150" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K150" s="8">
-        <v>80</v>
-      </c>
-      <c r="L150" s="4">
-        <v>2055</v>
-      </c>
-    </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A151" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="B151" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="C151" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="D151" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="E151" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F151" s="4">
-        <v>100</v>
-      </c>
-      <c r="G151" s="6">
-        <v>2055</v>
-      </c>
-      <c r="H151" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="I151" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="J151" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K151" s="8">
-        <v>20</v>
-      </c>
-      <c r="L151" s="4">
-        <v>2005</v>
-      </c>
-    </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A152" s="4"/>
-      <c r="B152" s="4"/>
-      <c r="C152" s="4"/>
-      <c r="D152" s="5"/>
-      <c r="E152" s="4"/>
-      <c r="F152" s="4"/>
-      <c r="G152" s="6"/>
-      <c r="H152" s="4"/>
-      <c r="I152" s="4"/>
-      <c r="J152" s="7"/>
-      <c r="K152" s="9"/>
-      <c r="L152" s="4"/>
-    </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A153" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="B153" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="C153" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D153" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="E153" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F153" s="14">
-        <f>SUM($K$153:$K$161)</f>
-        <v>76.335000000000008</v>
-      </c>
-      <c r="G153" s="15">
-        <v>2055</v>
-      </c>
-      <c r="H153" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="I153" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="J153" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K153" s="8">
-        <v>12.5</v>
-      </c>
-      <c r="L153" s="15">
-        <v>2055</v>
-      </c>
-    </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A154" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="B154" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="C154" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D154" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="E154" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F154" s="14">
-        <f t="shared" ref="F154:F161" si="0">SUM($K$153:$K$161)</f>
-        <v>76.335000000000008</v>
-      </c>
-      <c r="G154" s="15">
-        <v>2055</v>
-      </c>
-      <c r="H154" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="I154" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="J154" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K154" s="8">
-        <v>0</v>
-      </c>
-      <c r="L154" s="15">
-        <v>2055</v>
-      </c>
-    </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A155" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="B155" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="C155" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D155" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="E155" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F155" s="14">
-        <f t="shared" si="0"/>
-        <v>76.335000000000008</v>
-      </c>
-      <c r="G155" s="15">
-        <v>2055</v>
-      </c>
-      <c r="H155" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="I155" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="J155" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K155" s="8">
-        <v>0</v>
-      </c>
-      <c r="L155" s="15">
-        <v>2055</v>
-      </c>
-    </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A156" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="B156" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="C156" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D156" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="E156" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F156" s="14">
-        <f t="shared" si="0"/>
-        <v>76.335000000000008</v>
-      </c>
-      <c r="G156" s="15">
-        <v>2055</v>
-      </c>
-      <c r="H156" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="I156" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="J156" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K156" s="8">
-        <v>0</v>
-      </c>
-      <c r="L156" s="15">
-        <v>2055</v>
-      </c>
-    </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A157" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="B157" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="C157" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D157" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="E157" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F157" s="14">
-        <f t="shared" si="0"/>
-        <v>76.335000000000008</v>
-      </c>
-      <c r="G157" s="15">
-        <v>2055</v>
-      </c>
-      <c r="H157" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="I157" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="J157" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K157" s="8">
-        <v>10</v>
-      </c>
-      <c r="L157" s="15">
-        <v>2055</v>
-      </c>
-    </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A158" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="B158" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="C158" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D158" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="E158" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F158" s="14">
-        <f t="shared" si="0"/>
-        <v>76.335000000000008</v>
-      </c>
-      <c r="G158" s="15">
-        <v>2055</v>
-      </c>
-      <c r="H158" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I158" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="J158" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K158" s="9">
-        <v>0.83499999999999996</v>
-      </c>
-      <c r="L158" s="15">
-        <v>2055</v>
-      </c>
-    </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A159" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="B159" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="C159" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D159" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="E159" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F159" s="14">
-        <f t="shared" si="0"/>
-        <v>76.335000000000008</v>
-      </c>
-      <c r="G159" s="15">
-        <v>2055</v>
-      </c>
-      <c r="H159" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="I159" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="J159" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K159" s="9">
-        <v>32</v>
-      </c>
-      <c r="L159" s="15">
-        <v>2055</v>
-      </c>
-    </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A160" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="B160" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="C160" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D160" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="E160" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F160" s="14">
-        <f t="shared" si="0"/>
-        <v>76.335000000000008</v>
-      </c>
-      <c r="G160" s="15">
-        <v>2055</v>
-      </c>
-      <c r="H160" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="I160" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="J160" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K160" s="9">
-        <v>6</v>
-      </c>
-      <c r="L160" s="4">
-        <v>2035</v>
-      </c>
-    </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A161" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="B161" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="C161" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D161" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="E161" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F161" s="14">
-        <f t="shared" si="0"/>
-        <v>76.335000000000008</v>
-      </c>
-      <c r="G161" s="15">
-        <v>2055</v>
-      </c>
-      <c r="H161" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="I161" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="J161" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K161" s="8">
-        <v>15</v>
-      </c>
-      <c r="L161" s="4">
-        <v>2035</v>
-      </c>
-    </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A162" s="4"/>
-      <c r="B162" s="4"/>
-      <c r="C162" s="4"/>
-      <c r="D162" s="4"/>
-      <c r="E162" s="4"/>
-      <c r="F162" s="4"/>
-      <c r="G162" s="6"/>
-      <c r="H162" s="4"/>
-      <c r="I162" s="4"/>
-      <c r="J162" s="7"/>
-      <c r="K162" s="9"/>
-      <c r="L162" s="4"/>
-    </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A163" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="B163" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="C163" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="D163" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="E163" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F163" s="4">
-        <v>100</v>
-      </c>
-      <c r="G163" s="15">
-        <v>2055</v>
-      </c>
-      <c r="H163" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="I163" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="J163" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K163" s="8">
-        <v>40</v>
-      </c>
-      <c r="L163" s="15">
-        <v>2055</v>
-      </c>
-    </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A164" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="B164" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="C164" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="D164" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="E164" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F164" s="4">
-        <v>100</v>
-      </c>
-      <c r="G164" s="15">
-        <v>2055</v>
-      </c>
-      <c r="H164" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I164" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="J164" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K164" s="8">
-        <v>0.9</v>
-      </c>
-      <c r="L164" s="15">
-        <v>2055</v>
-      </c>
-    </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A165" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="B165" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="C165" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="D165" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="E165" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F165" s="4">
-        <v>100</v>
-      </c>
-      <c r="G165" s="15">
-        <v>2055</v>
-      </c>
-      <c r="H165" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="I165" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="J165" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K165" s="8">
-        <v>40</v>
-      </c>
-      <c r="L165" s="15">
-        <v>2055</v>
-      </c>
-    </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A166" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="B166" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="C166" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="D166" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="E166" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F166" s="4">
-        <v>100</v>
-      </c>
-      <c r="G166" s="15">
-        <v>2055</v>
-      </c>
-      <c r="H166" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="I166" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="J166" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K166" s="8">
-        <v>2</v>
-      </c>
-      <c r="L166" s="4">
-        <v>2005</v>
-      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1">

</xml_diff>